<commit_message>
changed website to kayak.com, homepage finished
</commit_message>
<xml_diff>
--- a/Resources/Book1.xlsx
+++ b/Resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tavis\OneDrive\Desktop\skyscanner\skyscanner\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37DA2CF-E203-40B0-9F27-B08DDBC5536F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612E087-3C6D-47C2-BB3C-1161845ABD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,13 +437,13 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -537,7 +537,7 @@
         <v>45282</v>
       </c>
       <c r="E3" s="2">
-        <v>45301</v>
+        <v>45303</v>
       </c>
       <c r="F3">
         <v>1</v>

</xml_diff>

<commit_message>
first search configuration fully controlled
</commit_message>
<xml_diff>
--- a/Resources/Book1.xlsx
+++ b/Resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tavis\OneDrive\Desktop\skyscanner\skyscanner\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612E087-3C6D-47C2-BB3C-1161845ABD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC856D0-41FC-4D03-A43C-2B32C57EB4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>From</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>19:00:00</t>
+  </si>
+  <si>
+    <t>UKR</t>
+  </si>
+  <si>
+    <t>BLG</t>
+  </si>
+  <si>
+    <t>SPN</t>
   </si>
 </sst>
 </file>
@@ -434,356 +443,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45265</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45283</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45292</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45323</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45282</v>
-      </c>
-      <c r="E3" s="2">
-        <v>45303</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="M3">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44927</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45291</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2">
-        <v>45251</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13">
+      <c r="L7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automatization finished, scraping logic left
</commit_message>
<xml_diff>
--- a/Resources/Book1.xlsx
+++ b/Resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tavis\OneDrive\Desktop\skyscanner\skyscanner\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC856D0-41FC-4D03-A43C-2B32C57EB4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5961E8-FB5F-45AE-A649-B88477D8209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,12 +446,13 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -629,5 +630,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished need to test
</commit_message>
<xml_diff>
--- a/Resources/Book1.xlsx
+++ b/Resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tavis\OneDrive\Desktop\skyscanner\skyscanner\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E659DA10-1295-4647-8BEB-53F4B2C57E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613EEFEB-97CF-4CC0-AE83-8A621D5C4B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>Provider</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>FRA</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>BLN</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -437,12 +437,13 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -480,15 +481,15 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>45323</v>
@@ -500,22 +501,22 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>70</v>
       </c>
       <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -523,10 +524,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>45261</v>
@@ -536,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -544,10 +545,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2">
         <v>45291</v>
@@ -559,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -567,10 +568,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>45250</v>
@@ -580,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -588,10 +589,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>45240</v>
@@ -601,13 +602,14 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>